<commit_message>
dataprovide for login failed due to null pointer exception
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hubspot/testdata/apptestdata.xlsx
+++ b/src/main/java/com/qa/hubspot/testdata/apptestdata.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NaveenKhunteta/Documents/workspace/MarchPOMSeries/src/main/java/com/qa/hubspot/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharat/eclipse-workspace/MarchPOMSeries_bharat/src/main/java/com/qa/hubspot/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="900" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="1540" yWindow="900" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginPage" sheetId="2" r:id="rId1"/>
+    <sheet name="contacts" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>email</t>
   </si>
@@ -100,13 +97,28 @@
   </si>
   <si>
     <t>Eng Mngr</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>&amp;@#$#$@</t>
+  </si>
+  <si>
+    <t>Auth@Bha!</t>
+  </si>
+  <si>
+    <t>pussharma@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +130,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,14 +166,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,9 +452,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -527,16 +595,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
excel sheet name updated
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hubspot/testdata/apptestdata.xlsx
+++ b/src/main/java/com/qa/hubspot/testdata/apptestdata.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="1540" yWindow="900" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginPage" sheetId="2" r:id="rId1"/>
+    <sheet name="login" sheetId="2" r:id="rId1"/>
     <sheet name="contacts" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>